<commit_message>
Atualização flowMap religa (PF)
</commit_message>
<xml_diff>
--- a/maps/Religa(POSFAMILIA)/exportedScenarios/Religa(Pós-Família) Scenarios.xlsx
+++ b/maps/Religa(POSFAMILIA)/exportedScenarios/Religa(Pós-Família) Scenarios.xlsx
@@ -1001,12 +1001,12 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Sucesso na Consulta de Dados
 * Navegação Reduzida
 * Sucesso no billing
 Quer pacote adicional
-Encaminha para o Fluxo de Contratação de Pacotes.</t>
+Encaminha para o ATH.</t>
   </si>
   <si>
     <t>1 - Chamada é encaminhada para a URA Cognitiva;
@@ -1014,7 +1014,7 @@
 3 - A URA Cognitiva pergunta se o usuário está com dificuldade para usar os serviços;
 4 - A URA Cognitiva pergunta em qual serviço o usuário está com dificuldades/problemas;
 5 - A URA Cognitiva informa que a velocidade está reduzida e a data de renovação;
-6 - URA entra no fluxo de contratação de pacotes.</t>
+6 - URA informa que vai tranferir para o ATH.</t>
   </si>
   <si>
     <t>07.047</t>
@@ -1022,7 +1022,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Sucesso na Consulta de Dados
 * Navegação Reduzida
 * Sucesso no billing
@@ -1043,12 +1043,12 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Sucesso na Consulta de Dados
 * Navegação Reduzida
 * Falha no billing
 Quer pacote adicional
-Encaminha para o Fluxo de Contratação de Pacotes.</t>
+Encaminha para o ATH.</t>
   </si>
   <si>
     <t>1 - Chamada é encaminhada para a URA Cognitiva;
@@ -1056,7 +1056,7 @@
 3 - A URA Cognitiva pergunta se o usuário está com dificuldade para usar os serviços;
 4 - A URA Cognitiva pergunta em qual serviço o usuário está com dificuldades/problemas;
 5 - A URA Cognitiva pergunta se o usuário quer saber mais sobre os pacotes adicionais;
-6 - URA entra no fluxo de contratação de pacotes.</t>
+6 - URA informa que vai tranferir para o ATH.</t>
   </si>
   <si>
     <t>07.049</t>
@@ -1064,7 +1064,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Sucesso na Consulta de Dados
 * Navegação Reduzida
 * Falha no billing
@@ -1085,7 +1085,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Sucesso na Consulta de Dados
 * Navegação Normal
 Quer falar com ATH
@@ -1106,7 +1106,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Sucesso na Consulta de Dados
 * Navegação Normal
 Quer continuar na URA
@@ -1130,7 +1130,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Sucesso na Consulta de Dados
 * Navegação Normal
 Quer continuar na URA
@@ -1154,7 +1154,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Sucesso na Consulta de Dados
 * Navegação Normal
 Quer continuar na URA
@@ -1177,7 +1177,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Sucesso na Consulta de Dados
 * Navegação Normal
 Quer continuar na URA
@@ -1203,7 +1203,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Sucesso na Consulta de Dados
 * Navegação Normal
 Quer continuar na URA
@@ -1229,7 +1229,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Falha na Consulta de Dados
 Já reiniciou
 * Sucesso no Envio do Guia
@@ -1249,7 +1249,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Falha na Consulta de Dados
 Já reiniciou
 * Falha no Envio do Guia
@@ -1269,7 +1269,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Falha na Consulta de Dados
 Não reiniciou
 Aceita Reiniciar</t>
@@ -1288,7 +1288,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Falha na Consulta de Dados
 Não reiniciou
 Não quer reiniciar
@@ -1310,7 +1310,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. na Internet
+Problema na Internet
 * Falha na Consulta de Dados
 Não reiniciou
 Não quer reiniciar
@@ -1332,7 +1332,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. nas ligações
+Problema nas ligações
 Quer falar com ATH
 Encaminha para o ATH.</t>
   </si>
@@ -1349,7 +1349,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. nas ligações
+Problema nas ligações
 Quer continuar na URA
 Já reiniciou
 * Sucesso no Envio do Guia
@@ -1361,7 +1361,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. nas ligações
+Problema nas ligações
 Quer continuar na URA
 Já reiniciou
 * Falha no Envio do Guia
@@ -1373,7 +1373,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. nas ligações
+Problema nas ligações
 Quer continuar na URA
 Não reiniciou
 Aceita Reiniciar</t>
@@ -1384,7 +1384,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. nas ligações
+Problema nas ligações
 Quer continuar na URA
 Não reiniciou
 Não quer reiniciar
@@ -1397,7 +1397,7 @@
   <si>
     <t>Quer fazer Religa
 Está enfrentando dificuldade
-Prob. nas ligações
+Problema nas ligações
 Quer continuar na URA
 Não reiniciou
 Não quer reiniciar

</xml_diff>